<commit_message>
added file download and modified export excel file
</commit_message>
<xml_diff>
--- a/ExportImport/Cinema.Web/Files/member.xlsx
+++ b/ExportImport/Cinema.Web/Files/member.xlsx
@@ -12,10 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>MemberId</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>FullName</t>
   </si>
@@ -23,10 +20,10 @@
     <t>Address</t>
   </si>
   <si>
-    <t>MovieId</t>
+    <t>MoviesRented</t>
   </si>
   <si>
-    <t>SalutationId</t>
+    <t>Salutation</t>
   </si>
   <si>
     <t>Sandy</t>
@@ -35,10 +32,25 @@
     <t>First Street Plot 4</t>
   </si>
   <si>
+    <t>Daddy's Little Girls</t>
+  </si>
+  <si>
+    <t>Ms</t>
+  </si>
+  <si>
+    <t>Clash of the Titans 2</t>
+  </si>
+  <si>
     <t>John</t>
   </si>
   <si>
     <t>Second Street Plot 5</t>
+  </si>
+  <si>
+    <t>Forgetting Sarah Marshal</t>
+  </si>
+  <si>
+    <t>Mr</t>
   </si>
   <si>
     <t>Jonet Jones</t>
@@ -90,7 +102,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -109,13 +121,10 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="0">
-        <v>17017</v>
+      <c r="A2" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>5</v>
@@ -123,79 +132,64 @@
       <c r="C2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0">
-        <v>2</v>
-      </c>
-      <c r="E2" s="0">
-        <v>2</v>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0">
-        <v>17018</v>
+      <c r="A3" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
-      <c r="D3" s="0">
-        <v>1</v>
-      </c>
-      <c r="E3" s="0">
-        <v>2</v>
+      <c r="D3" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0">
-        <v>17019</v>
+      <c r="A4" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
-      <c r="D4" s="0">
-        <v>3</v>
-      </c>
-      <c r="E4" s="0">
-        <v>1</v>
+      <c r="D4" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0">
-        <v>17020</v>
+      <c r="A5" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="0">
-        <v>1</v>
-      </c>
-      <c r="E5" s="0">
-        <v>1</v>
+      <c r="D5" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="0">
-        <v>17021</v>
+      <c r="A6" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
-      <c r="D6" s="0">
-        <v>2</v>
-      </c>
-      <c r="E6" s="0">
-        <v>1</v>
+      <c r="D6" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified import excel file
</commit_message>
<xml_diff>
--- a/ExportImport/Cinema.Web/Files/member.xlsx
+++ b/ExportImport/Cinema.Web/Files/member.xlsx
@@ -102,7 +102,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -192,6 +192,76 @@
         <v>12</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>